<commit_message>
Minor Update to data
</commit_message>
<xml_diff>
--- a/Vermintide 2 Chest Drop Rates.xlsx
+++ b/Vermintide 2 Chest Drop Rates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjang\Documents\Vermintide Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5098C3-46E8-43ED-AFF5-34E320D17467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A91640-89B3-4F3A-95C3-19E9037C53BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,7 +653,7 @@
   <dimension ref="A1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +728,9 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F6" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="G6" t="s">
         <v>60</v>
       </c>
@@ -909,9 +912,6 @@
       </c>
       <c r="D20">
         <v>2</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="G20" t="s">
         <v>26</v>

</xml_diff>